<commit_message>
new price schema working
</commit_message>
<xml_diff>
--- a/db/dummydata/2_service_charges.xlsx
+++ b/db/dummydata/2_service_charges.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="40">
   <si>
     <t>EFFECTIVE_DATE</t>
   </si>
@@ -106,10 +106,31 @@
     <t>LOO1</t>
   </si>
   <si>
-    <t>VEO1</t>
+    <t>SIO1</t>
   </si>
   <si>
-    <t>MAO1</t>
+    <t>GOA1</t>
+  </si>
+  <si>
+    <t>SHA1</t>
+  </si>
+  <si>
+    <t>HAA1</t>
+  </si>
+  <si>
+    <t>ROA1</t>
+  </si>
+  <si>
+    <t>MUA1</t>
+  </si>
+  <si>
+    <t>NIA1</t>
+  </si>
+  <si>
+    <t>LOA1</t>
+  </si>
+  <si>
+    <t>SIA1</t>
   </si>
 </sst>
 </file>
@@ -1154,10 +1175,10 @@
         <v>43465.0</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
       </c>
       <c r="E10">
         <v>165.0</v>
@@ -1168,8 +1189,8 @@
       <c r="G10">
         <v>395.0</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>24</v>
+      <c r="H10" t="s">
+        <v>22</v>
       </c>
       <c r="I10">
         <v>50.0</v>
@@ -1186,26 +1207,26 @@
       <c r="M10">
         <v>5.0</v>
       </c>
-      <c r="N10" s="7" t="s">
-        <v>24</v>
+      <c r="N10" t="s">
+        <v>22</v>
       </c>
       <c r="O10">
         <v>400.0</v>
       </c>
-      <c r="P10" s="7" t="s">
-        <v>24</v>
+      <c r="P10" t="s">
+        <v>22</v>
       </c>
       <c r="Q10">
         <v>50.0</v>
       </c>
-      <c r="R10" s="7" t="s">
-        <v>24</v>
+      <c r="R10" t="s">
+        <v>22</v>
       </c>
       <c r="S10">
         <v>625.0</v>
       </c>
-      <c r="T10" s="7" t="s">
-        <v>24</v>
+      <c r="T10" t="s">
+        <v>22</v>
       </c>
       <c r="U10">
         <v>675.0</v>
@@ -1216,32 +1237,32 @@
       <c r="W10">
         <v>25.0</v>
       </c>
-      <c r="X10" s="7" t="s">
-        <v>24</v>
+      <c r="X10" t="s">
+        <v>22</v>
       </c>
       <c r="Y10">
         <v>40.0</v>
       </c>
-      <c r="Z10" s="7" t="s">
-        <v>24</v>
+      <c r="Z10" t="s">
+        <v>22</v>
       </c>
       <c r="AA10" s="7">
         <v>5.0</v>
       </c>
-      <c r="AB10" s="7" t="s">
-        <v>24</v>
+      <c r="AB10" t="s">
+        <v>22</v>
       </c>
       <c r="AC10" s="7">
         <v>50.0</v>
       </c>
-      <c r="AD10" s="7" t="s">
-        <v>24</v>
+      <c r="AD10" t="s">
+        <v>22</v>
       </c>
       <c r="AE10" s="7">
         <v>25.0</v>
       </c>
-      <c r="AF10" s="7" t="s">
-        <v>24</v>
+      <c r="AF10" t="s">
+        <v>22</v>
       </c>
       <c r="AG10" s="7">
         <v>22.0</v>
@@ -1255,7 +1276,7 @@
         <v>43465.0</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>24</v>
@@ -1349,28 +1370,610 @@
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6">
+        <v>43101.0</v>
+      </c>
+      <c r="B12" s="6">
+        <v>43465.0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>165.0</v>
+      </c>
+      <c r="F12">
+        <v>395.0</v>
+      </c>
+      <c r="G12">
+        <v>395.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <v>50.0</v>
+      </c>
+      <c r="J12">
+        <v>50.0</v>
+      </c>
+      <c r="K12">
+        <v>50.0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12">
+        <v>5.0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12">
+        <v>400.0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12">
+        <v>50.0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12">
+        <v>625.0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12">
+        <v>675.0</v>
+      </c>
+      <c r="V12" t="s">
+        <v>23</v>
+      </c>
+      <c r="W12">
+        <v>25.0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y12">
+        <v>40.0</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC12" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE12" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG12" s="7">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="6">
+        <v>43101.0</v>
+      </c>
+      <c r="B13" s="6">
+        <v>43465.0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>165.0</v>
+      </c>
+      <c r="F13">
+        <v>395.0</v>
+      </c>
+      <c r="G13">
+        <v>395.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>50.0</v>
+      </c>
+      <c r="J13">
+        <v>50.0</v>
+      </c>
+      <c r="K13">
+        <v>50.0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <v>5.0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13">
+        <v>400.0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13">
+        <v>50.0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13">
+        <v>625.0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13">
+        <v>675.0</v>
+      </c>
+      <c r="V13" t="s">
+        <v>23</v>
+      </c>
+      <c r="W13">
+        <v>25.0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y13">
+        <v>40.0</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE13" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG13" s="7">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="6">
+        <v>43101.0</v>
+      </c>
+      <c r="B14" s="6">
+        <v>43465.0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>165.0</v>
+      </c>
+      <c r="F14">
+        <v>395.0</v>
+      </c>
+      <c r="G14">
+        <v>395.0</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14">
+        <v>50.0</v>
+      </c>
+      <c r="J14">
+        <v>50.0</v>
+      </c>
+      <c r="K14">
+        <v>50.0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14">
+        <v>5.0</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14">
+        <v>400.0</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14">
+        <v>50.0</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14">
+        <v>625.0</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U14">
+        <v>675.0</v>
+      </c>
+      <c r="V14" t="s">
+        <v>24</v>
+      </c>
+      <c r="W14">
+        <v>25.0</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y14">
+        <v>40.0</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="AB14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="AD14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG14" s="7">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="6">
+        <v>43101.0</v>
+      </c>
+      <c r="B15" s="6">
+        <v>43465.0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>165.0</v>
+      </c>
+      <c r="F15">
+        <v>395.0</v>
+      </c>
+      <c r="G15">
+        <v>395.0</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15">
+        <v>50.0</v>
+      </c>
+      <c r="J15">
+        <v>50.0</v>
+      </c>
+      <c r="K15">
+        <v>50.0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15">
+        <v>5.0</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15">
+        <v>400.0</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15">
+        <v>50.0</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S15">
+        <v>625.0</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U15">
+        <v>675.0</v>
+      </c>
+      <c r="V15" t="s">
+        <v>24</v>
+      </c>
+      <c r="W15">
+        <v>25.0</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y15">
+        <v>40.0</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE15" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="AF15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG15" s="7">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="6">
+        <v>43101.0</v>
+      </c>
+      <c r="B16" s="6">
+        <v>43465.0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>165.0</v>
+      </c>
+      <c r="F16">
+        <v>395.0</v>
+      </c>
+      <c r="G16">
+        <v>395.0</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>50.0</v>
+      </c>
+      <c r="J16">
+        <v>50.0</v>
+      </c>
+      <c r="K16">
+        <v>50.0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16">
+        <v>5.0</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16">
+        <v>400.0</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16">
+        <v>50.0</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16">
+        <v>625.0</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U16">
+        <v>675.0</v>
+      </c>
+      <c r="V16" t="s">
+        <v>24</v>
+      </c>
+      <c r="W16">
+        <v>25.0</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y16">
+        <v>40.0</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA16" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC16" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="AD16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE16" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="AF16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG16" s="7">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="6">
+        <v>43101.0</v>
+      </c>
+      <c r="B17" s="6">
+        <v>43465.0</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>165.0</v>
+      </c>
+      <c r="F17">
+        <v>395.0</v>
+      </c>
+      <c r="G17">
+        <v>395.0</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17">
+        <v>50.0</v>
+      </c>
+      <c r="J17">
+        <v>50.0</v>
+      </c>
+      <c r="K17">
+        <v>50.0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17">
+        <v>5.0</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17">
+        <v>400.0</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17">
+        <v>50.0</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S17">
+        <v>625.0</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U17">
+        <v>675.0</v>
+      </c>
+      <c r="V17" t="s">
+        <v>24</v>
+      </c>
+      <c r="W17">
+        <v>25.0</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y17">
+        <v>40.0</v>
+      </c>
+      <c r="Z17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA17" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC17" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE17" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="AF17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG17" s="7">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="6"/>

</xml_diff>